<commit_message>
Adding Screenshots to Testng
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>firstName</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Youssef</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
   </si>
 </sst>
 </file>
@@ -356,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,8 +380,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -384,6 +393,9 @@
       </c>
       <c r="C2">
         <v>11725</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding hashtable to parameterize
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22530" windowHeight="7170"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22530" windowHeight="7170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -82,19 +82,16 @@
     <t>runmode</t>
   </si>
   <si>
+    <t>bankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>addCustomerTest</t>
+  </si>
+  <si>
+    <t>openAccountTest</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>bankManagerLoginTest</t>
-  </si>
-  <si>
-    <t>addCustomerTest</t>
-  </si>
-  <si>
-    <t>openAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -414,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,26 +430,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -462,15 +459,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +480,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -497,8 +497,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -511,8 +514,11 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -525,8 +531,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -538,6 +547,9 @@
       </c>
       <c r="D5" t="s">
         <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -551,7 +563,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Parameterize Browser election in runtime
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>firstName</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>openAccountTest</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>Y</t>
@@ -433,7 +436,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -441,7 +444,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +452,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -498,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -532,7 +535,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>